<commit_message>
updates project 3 requirements
</commit_message>
<xml_diff>
--- a/.DOCUMENTATION/Requirements/Project 3 Requirements.xlsx
+++ b/.DOCUMENTATION/Requirements/Project 3 Requirements.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="121">
   <si>
     <t>Reference Story Label</t>
   </si>
@@ -38,34 +38,46 @@
     <t>Added a feature where specific sound effects played upon certain event handlers triggering on a Javascript webpage. This was extremely simple and easy to replicate multiple times for various contexts.</t>
   </si>
   <si>
-    <t>Mine Input</t>
+    <t>FizzBuzz</t>
+  </si>
+  <si>
+    <t>Common computer science exercise</t>
+  </si>
+  <si>
+    <t>A simple function that returns a string following a pattern based on divisibility rules of the inputted value n.</t>
+  </si>
+  <si>
+    <t>Reading a file</t>
+  </si>
+  <si>
+    <t>EECS168 Labs</t>
+  </si>
+  <si>
+    <t>Reading a file into your script using Python. Involves reading the file name and splicing the returned string(s) to be handled by the program.</t>
+  </si>
+  <si>
+    <t>Linked List Data Structure</t>
+  </si>
+  <si>
+    <t>EECS330; Linked List Lab</t>
+  </si>
+  <si>
+    <t>Implements a basic linked list data structure in Python, with common helper methods and insert/delete methods.</t>
+  </si>
+  <si>
+    <t>Basic Client/Server setup in Rust</t>
+  </si>
+  <si>
+    <t>Personal Project</t>
+  </si>
+  <si>
+    <t>Implements a client and server skeleton in Rust following the tutorial in the Rust book.</t>
+  </si>
+  <si>
+    <t>Generate Minefield Array</t>
   </si>
   <si>
     <t>EECS581; Minesweeper Part 1</t>
-  </si>
-  <si>
-    <t>Added an input box that contained a list of values corresponding to mine count. Input was taken, assigned to a variable and called in a function to generate a minefield with the set amount of mines.</t>
-  </si>
-  <si>
-    <t>Game Info</t>
-  </si>
-  <si>
-    <t>Added html element and javascript alerts to make user interaction with the program easier via more communication of allowed actions.</t>
-  </si>
-  <si>
-    <t>Reveal Effect</t>
-  </si>
-  <si>
-    <t>Added a left click event listener to each mine that only triggers when the click is valid, that disables the mine and changes the style after the mine is clicked, while also revealing the number of adjacent mines.</t>
-  </si>
-  <si>
-    <t>Easy Bot Difficulty</t>
-  </si>
-  <si>
-    <t>Implemented an automatic game option in Minesweeper where the bot clicks any random tile that is not flagged and has not already been revealed (unrevealed tiles). Involved random number generation and basic programming.</t>
-  </si>
-  <si>
-    <t>Generate Minefield Array</t>
   </si>
   <si>
     <t>Generated an array based on the number of mines, each non-mine space getting set to a number based on the proximity of mines in a 3x3 grid. Involved array filling, randomization, and iteration checks.</t>
@@ -118,10 +130,13 @@
     <t>Implemented an algorithm to play MineSweeper based on revealed tiles, where it would go through every cell and flag/click cells based on the proximity of hidden cells nearby. Involved game sense with dom query selectors and iteration.</t>
   </si>
   <si>
-    <t>Flagging Event Handlers</t>
-  </si>
-  <si>
-    <t>Implemented flagging in Minesweeper using Javascript. Involved multiple event handlers including some for determining cursor's coordinates on screen and for detecting the press of a specific key.</t>
+    <t>Dijkstra's Algorithm</t>
+  </si>
+  <si>
+    <t>EECS330; Weighted Graphs Lab</t>
+  </si>
+  <si>
+    <t>Implemented Djikstra's algorithm in Python, a somewhat complex algorithm involving techniques such as recursion, BFS traversal and backtracking to find the shortest path between other nodes in a weighted graph.</t>
   </si>
   <si>
     <t>Minesweeper Game State</t>
@@ -130,10 +145,10 @@
     <t>Implemented game state mechanics for Minesweeper using Javascript, including tracking game over and victory conditions, as well as keeping track of the current state (e.g. playing, uninitialized, game over, etc.) with various state transitions.</t>
   </si>
   <si>
-    <t>Git/GitHub Workflow</t>
-  </si>
-  <si>
-    <t>Utilize a Git/GitHub environment where coders create branches and merge pull requests to contribute to a GitHub repository. Involves pulling, pushing, and a lot of merge conflicts.</t>
+    <t>Basic GUI Calculator in Python</t>
+  </si>
+  <si>
+    <t>Created a basic arithmetic calculator using Python's tkinter package. Implemented addition, subtraction, multiplication, division and supported floats.</t>
   </si>
   <si>
     <t>Path Traversal</t>
@@ -157,9 +172,6 @@
     <t>Nim Game in C</t>
   </si>
   <si>
-    <t>Personal Project</t>
-  </si>
-  <si>
     <t>Implements Nim Game in C allowing a user to play against another human locally or agasint a bot opponent that plays optimally.</t>
   </si>
   <si>
@@ -196,15 +208,6 @@
     <t>Displayed SQL entries on a website using PHP controllers, web routes, and models. Added form submission and validation to delete entries, add new ones, and modify existing entries.</t>
   </si>
   <si>
-    <t>Job Implementation</t>
-  </si>
-  <si>
-    <t>EECS678; Quash Project</t>
-  </si>
-  <si>
-    <t>Handled a simulated flow of jobs being created, executed, put into background tasks and completed in a Quash project. Complexity came from both the abstractness of the job conceptually and specific algorithms and techniques used to implement it.</t>
-  </si>
-  <si>
     <t>Static Analysis Engine</t>
   </si>
   <si>
@@ -286,6 +289,9 @@
     <t>8: (Stretch Goal) Completely Optional</t>
   </si>
   <si>
+    <t>User can access a shop page to see items for purchase</t>
+  </si>
+  <si>
     <t>User can buy items from the shop using coins</t>
   </si>
   <si>
@@ -343,21 +349,9 @@
     <t>User can gets coins from consistently doing tasks (streak/Journey/Skill streak)</t>
   </si>
   <si>
-    <t>User can ask the COACH for task ideas</t>
-  </si>
-  <si>
     <t>User can change/customize the UI/Interface (bought with coins)</t>
   </si>
   <si>
-    <t>User can create a task with a timer that the user can start, and the task will complete when timer is done</t>
-  </si>
-  <si>
-    <t>User can create a task with a word count that will open a text box, and will complete when the user reaches the word count and submits</t>
-  </si>
-  <si>
-    <t>User can create an exercise/stretch task – which is like a timer task but displays exercises/stretches to do</t>
-  </si>
-  <si>
     <t>User can customize the COACH’s dialogue (bought with coins)</t>
   </si>
   <si>
@@ -367,19 +361,34 @@
     <t>User can "level up" a Journey/Skill</t>
   </si>
   <si>
-    <t>User can unlock Achievements</t>
-  </si>
-  <si>
     <t>User can import/create a custom COACH with images/animations/dialogue</t>
   </si>
   <si>
-    <t>User can see a RELATIONSHIP METER for the COACH</t>
-  </si>
-  <si>
-    <t>User can buy/give COACH gifts and food</t>
-  </si>
-  <si>
-    <t>User can go ON A DATE with COACH</t>
+    <t>Creation of an inventory</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Sum of Story Points Per Sprint</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint Final</t>
   </si>
 </sst>
 </file>
@@ -730,15 +739,15 @@
         <v>1.0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3">
         <v>4.0</v>
@@ -747,15 +756,15 @@
         <v>2.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3">
         <v>5.0</v>
@@ -764,15 +773,15 @@
         <v>2.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3">
         <v>6.0</v>
@@ -781,15 +790,15 @@
         <v>2.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3">
         <v>7.0</v>
@@ -798,15 +807,15 @@
         <v>2.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3">
         <v>8.0</v>
@@ -815,15 +824,15 @@
         <v>3.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3">
         <v>9.0</v>
@@ -832,15 +841,15 @@
         <v>3.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3">
         <v>10.0</v>
@@ -852,12 +861,12 @@
         <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3">
         <v>11.0</v>
@@ -866,15 +875,15 @@
         <v>5.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3">
         <v>12.0</v>
@@ -883,15 +892,15 @@
         <v>5.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B14" s="3">
         <v>13.0</v>
@@ -900,15 +909,15 @@
         <v>5.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3">
         <v>14.0</v>
@@ -917,15 +926,15 @@
         <v>5.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3">
         <v>15.0</v>
@@ -934,15 +943,15 @@
         <v>8.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3">
         <v>16.0</v>
@@ -951,15 +960,15 @@
         <v>8.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B18" s="3">
         <v>17.0</v>
@@ -968,15 +977,15 @@
         <v>8.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B19" s="3">
         <v>18.0</v>
@@ -985,15 +994,15 @@
         <v>13.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B20" s="3">
         <v>19.0</v>
@@ -1002,15 +1011,15 @@
         <v>13.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B21" s="3">
         <v>20.0</v>
@@ -1019,15 +1028,15 @@
         <v>13.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B22" s="3">
         <v>21.0</v>
@@ -1036,15 +1045,15 @@
         <v>21.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3">
         <v>22.0</v>
@@ -1053,27 +1062,10 @@
         <v>21.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="C24" s="3">
-        <v>21.0</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1100,22 +1092,22 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">
@@ -1123,7 +1115,7 @@
         <v>0.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
@@ -1135,7 +1127,7 @@
         <v>1.0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
@@ -1143,7 +1135,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" s="3">
         <v>1.0</v>
@@ -1155,7 +1147,7 @@
         <v>1.0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4">
@@ -1163,7 +1155,7 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" s="3">
         <v>1.0</v>
@@ -1175,7 +1167,7 @@
         <v>1.0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
@@ -1183,7 +1175,7 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3">
         <v>2.0</v>
@@ -1195,7 +1187,7 @@
         <v>1.0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
@@ -1203,7 +1195,7 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" s="3">
         <v>3.0</v>
@@ -1215,7 +1207,7 @@
         <v>2.0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
@@ -1225,7 +1217,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="6"/>
       <c r="G7" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
@@ -1233,7 +1225,7 @@
         <v>5.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C8" s="3">
         <v>1.0</v>
@@ -1245,7 +1237,7 @@
         <v>2.0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
@@ -1253,7 +1245,7 @@
         <v>6.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C9" s="3">
         <v>1.0</v>
@@ -1265,7 +1257,7 @@
         <v>2.0</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10">
@@ -1273,10 +1265,10 @@
         <v>7.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10" s="3">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="D10" s="3">
         <v>2.0</v>
@@ -1290,16 +1282,16 @@
         <v>8.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C11" s="3">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="D11" s="3">
         <v>2.0</v>
       </c>
       <c r="E11" s="3">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="12">
@@ -1307,10 +1299,10 @@
         <v>9.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C12" s="3">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="D12" s="3">
         <v>2.0</v>
@@ -1324,10 +1316,10 @@
         <v>10.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C13" s="3">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="D13" s="3">
         <v>2.0</v>
@@ -1341,16 +1333,16 @@
         <v>11.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C14" s="3">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="D14" s="3">
         <v>2.0</v>
       </c>
       <c r="E14" s="3">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="15">
@@ -1358,7 +1350,7 @@
         <v>12.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C15" s="3">
         <v>5.0</v>
@@ -1367,29 +1359,31 @@
         <v>2.0</v>
       </c>
       <c r="E15" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D16" s="3">
         <v>2.0</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="3">
-        <v>13.0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>3.0</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="6"/>
     </row>
     <row r="18">
@@ -1397,438 +1391,469 @@
         <v>14.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C18" s="3">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D18" s="3">
         <v>3.0</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="3"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="6"/>
+      <c r="A19" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="3">
-        <v>15.0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="3">
-        <v>13.0</v>
-      </c>
-      <c r="D20" s="3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
+        <v>16.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="3">
+        <v>21.0</v>
+      </c>
+      <c r="D21" s="3">
         <v>4.0</v>
       </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="3"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="6"/>
-      <c r="G21" s="2"/>
+      <c r="E21" s="3">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="3">
-        <v>16.0</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>5.0</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="6"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" s="3">
         <v>17.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C23" s="3">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D23" s="3">
         <v>5.0</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="D24" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="E24" s="6"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25">
       <c r="A25" s="3">
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C25" s="3">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="D25" s="3">
         <v>5.0</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C26" s="3">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="D26" s="3">
         <v>5.0</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C27" s="3">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="D27" s="3">
         <v>5.0</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="3">
-        <v>22.0</v>
+        <v>21.0</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C28" s="3">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D28" s="3">
         <v>5.0</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="3">
-        <v>23.0</v>
+        <v>22.0</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C29" s="3">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="D29" s="3">
         <v>5.0</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="3">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C30" s="3">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="D30" s="3">
         <v>5.0</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="3"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="3">
+        <v>24.0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3">
         <v>25.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C32" s="3">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D32" s="3">
-        <v>6.0</v>
-      </c>
-      <c r="E32" s="6"/>
+        <v>5.0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="3">
-        <v>26.0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="D33" s="3">
-        <v>6.0</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="6"/>
     </row>
     <row r="34">
       <c r="A34" s="3">
-        <v>27.0</v>
+        <v>26.0</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C34" s="3">
-        <v>13.0</v>
+        <v>2.0</v>
       </c>
       <c r="D34" s="3">
         <v>6.0</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="3"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="6"/>
+      <c r="A35" s="3">
+        <v>27.0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="3">
-        <v>28.0</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="D36" s="3">
-        <v>7.0</v>
-      </c>
+      <c r="A36" s="3"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
       <c r="E36" s="6"/>
     </row>
     <row r="37">
       <c r="A37" s="3">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C37" s="3">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="D37" s="3">
         <v>7.0</v>
       </c>
-      <c r="E37" s="6"/>
+      <c r="E37" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="3">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C38" s="3">
-        <v>13.0</v>
+        <v>8.0</v>
       </c>
       <c r="D38" s="3">
         <v>7.0</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="3">
-        <v>31.0</v>
-      </c>
-      <c r="B39" s="1" t="s">
+        <v>30.0</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>110</v>
       </c>
       <c r="C39" s="3">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="D39" s="3">
         <v>7.0</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="3">
-        <v>32.0</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="D40" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="E40" s="6"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
     </row>
     <row r="41">
       <c r="A41" s="3">
-        <v>33.0</v>
-      </c>
-      <c r="B41" s="2" t="s">
+        <v>31.0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="E41" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="3">
+        <v>32.0</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C41" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="D41" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="3">
-        <v>34.0</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="D42" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="3"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="C43" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D43" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="3">
-        <v>35.0</v>
+        <v>33.0</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C44" s="3">
-        <v>13.0</v>
-      </c>
-      <c r="D44" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="E44" s="3"/>
     </row>
     <row r="45">
       <c r="A45" s="3">
-        <v>36.0</v>
+        <v>34.0</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C45" s="3">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D45" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="E45" s="6"/>
+        <v>1.0</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="3">
-        <v>37.0</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="A46" s="3"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="3"/>
+      <c r="B47" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C46" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D46" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="3">
-        <v>38.0</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C47" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D47" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
+      <c r="B48" s="7">
+        <f>SUM(C2,C3,C4,C5)</f>
+        <v>5</v>
+      </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
     <row r="49">
-      <c r="A49" s="6"/>
-      <c r="B49" s="7"/>
+      <c r="A49" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="7">
+        <f>SUM(C6,C8,C9,C10,C12,C13,C21,C23)</f>
+        <v>42</v>
+      </c>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
     <row r="50">
-      <c r="A50" s="6"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" s="7">
+        <f>SUM(C11,C14,C15,C16,C18,C19,C25,C26,C27,C28,C29,C30,C31,C32,C34,C35,C37,C38,C39,C41,C43)</f>
+        <v>107</v>
+      </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
     <row r="51">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
+      <c r="A51" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" s="1">
+        <v>10.0</v>
+      </c>
       <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
+      <c r="D51" s="3"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52">
@@ -1840,28 +1865,24 @@
     </row>
     <row r="53">
       <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
     <row r="54">
       <c r="A54" s="6"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="6"/>
+      <c r="C54" s="3"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
     <row r="55">
       <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
       <c r="C55" s="6"/>
-      <c r="D55" s="3"/>
+      <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
     <row r="56">
       <c r="A56" s="6"/>
-      <c r="B56" s="7"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -1874,7 +1895,7 @@
     </row>
     <row r="58">
       <c r="A58" s="6"/>
-      <c r="C58" s="3"/>
+      <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
@@ -7548,30 +7569,6 @@
       <c r="D1003" s="6"/>
       <c r="E1003" s="6"/>
     </row>
-    <row r="1004">
-      <c r="A1004" s="6"/>
-      <c r="C1004" s="6"/>
-      <c r="D1004" s="6"/>
-      <c r="E1004" s="6"/>
-    </row>
-    <row r="1005">
-      <c r="A1005" s="6"/>
-      <c r="C1005" s="6"/>
-      <c r="D1005" s="6"/>
-      <c r="E1005" s="6"/>
-    </row>
-    <row r="1006">
-      <c r="A1006" s="6"/>
-      <c r="C1006" s="6"/>
-      <c r="D1006" s="6"/>
-      <c r="E1006" s="6"/>
-    </row>
-    <row r="1007">
-      <c r="A1007" s="6"/>
-      <c r="C1007" s="6"/>
-      <c r="D1007" s="6"/>
-      <c r="E1007" s="6"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>